<commit_message>
updated Code of Client Security hash
</commit_message>
<xml_diff>
--- a/Preethi/calculate_client_security_hash_2021_preethi/Data/Config.xlsx
+++ b/Preethi/calculate_client_security_hash_2021_preethi/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sridh\OneDrive\Documents\Rpa developer in 30days backup\Preethi\calculate_client_security_hash_2021_preethi\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4D88B6-E24A-4ECA-B73E-EDFA02907BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC79E457-474D-435D-8AFB-770807E43C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -579,7 +579,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -587,7 +587,7 @@
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -596,7 +596,7 @@
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1610,7 +1610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>